<commit_message>
Updated metadata injection spreadsheet
</commit_message>
<xml_diff>
--- a/content/evaluation/01_Fill_the_data_lake/data/Tower_logs_metadata.xlsx
+++ b/content/evaluation/01_Fill_the_data_lake/data/Tower_logs_metadata.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbuckallew\Documents\Big Data Sandbox\Data\Log File Metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbuckallew\Documents\Big Data Sandbox\Evaluation\01_Fill_the_data_lake\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13584" windowHeight="4524" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="callrecords_tower1" sheetId="1" r:id="rId1"/>
-    <sheet name="callrecords_tower2" sheetId="2" r:id="rId2"/>
-    <sheet name="callrecords_tower3" sheetId="3" r:id="rId3"/>
+    <sheet name="callrecords_tower1.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="callrecords_tower2.csv" sheetId="2" r:id="rId2"/>
+    <sheet name="callrecords_tower3.csv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>

</xml_diff>